<commit_message>
HTML version for webpage.
</commit_message>
<xml_diff>
--- a/due_dates.xlsx
+++ b/due_dates.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/80be582f19583417/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\OneDrive\Desktop\bureaucracy_undergrad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13C6E3DF-9E01-4942-A92C-2950D8266CDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{13C6E3DF-9E01-4942-A92C-2950D8266CDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A1AE1D42-083E-4D06-B988-38B13C1FF00A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{AB8CA921-76C0-4BD3-975C-015D17FBEAF7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">  Requirement </t>
   </si>
@@ -44,35 +44,53 @@
     <t xml:space="preserve"> Percent (\%) </t>
   </si>
   <si>
-    <t xml:space="preserve">  Participation </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Vignettes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Research Project </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Due Dates</t>
   </si>
   <si>
-    <t xml:space="preserve"> When Scheduled</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> By Wednesday, November 18</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> By Monday, December 7</t>
+    <t>Reflection Paper 1</t>
+  </si>
+  <si>
+    <t>Reflection Paper 2</t>
+  </si>
+  <si>
+    <t>Reflection Paper 3</t>
+  </si>
+  <si>
+    <t>Reflection Paper 4</t>
+  </si>
+  <si>
+    <t>Participation</t>
+  </si>
+  <si>
+    <t>Friday, September 18</t>
+  </si>
+  <si>
+    <t>Friday, October 9</t>
+  </si>
+  <si>
+    <t>Friday, November 13</t>
+  </si>
+  <si>
+    <t>Friday, December 11</t>
+  </si>
+  <si>
+    <t>Rolling Basis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,8 +116,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,11 +433,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1ED09AC-8BDA-462B-B369-4CF8B1CE9B16}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -431,52 +456,81 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
       <c r="C3">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>